<commit_message>
Model used for parameters 12/7/2017
</commit_message>
<xml_diff>
--- a/Studies/accuracy and number of sub HEX.xlsx
+++ b/Studies/accuracy and number of sub HEX.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="33">
   <si>
     <t>mH</t>
   </si>
@@ -26824,7 +26824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -27473,13 +27473,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB41"/>
+  <dimension ref="A1:AB52"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Y11" sqref="Y11"/>
+      <selection pane="bottomRight" activeCell="I49" sqref="A49:I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28320,7 +28320,7 @@
         <v>561.82229350921659</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f>A16/10</f>
         <v>1.0000000000000002E-12</v>
@@ -28371,7 +28371,7 @@
         <v>561.82229350921659</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002E-13</v>
@@ -28422,7 +28422,7 @@
         <v>561.82229351115836</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002E-14</v>
@@ -28473,7 +28473,7 @@
         <v>561.82229351115836</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000001E-15</v>
@@ -28524,7 +28524,7 @@
         <v>561.82229351116257</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000001E-16</v>
@@ -28575,7 +28575,7 @@
         <v>561.82229351115905</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -28625,7 +28625,7 @@
         <v>561.82229351115973</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>0.1</v>
       </c>
@@ -28653,6 +28653,14 @@
         <f>(G6-G$22)/G$22</f>
         <v>4.1049866093540721E-2</v>
       </c>
+      <c r="H25">
+        <f>ABS(F25)</f>
+        <v>2.8533750911036045E-2</v>
+      </c>
+      <c r="I25">
+        <f>ABS(G25)</f>
+        <v>4.1049866093540721E-2</v>
+      </c>
       <c r="K25">
         <f>K6</f>
         <v>5.9841394464340497E-3</v>
@@ -28677,6 +28685,14 @@
         <f>(P6-P$22)/P$22</f>
         <v>-1.3566726742124601E-2</v>
       </c>
+      <c r="Q25">
+        <f>ABS(O25)</f>
+        <v>4.7067750080677659E-3</v>
+      </c>
+      <c r="R25">
+        <f>ABS(P25)</f>
+        <v>1.3566726742124601E-2</v>
+      </c>
       <c r="W25">
         <f>W6</f>
         <v>4.773459938926683E-2</v>
@@ -28689,8 +28705,16 @@
         <f>(Y6-Y$22)/Y$22</f>
         <v>-1.6807524253678666E-2</v>
       </c>
+      <c r="Z25">
+        <f>ABS(X25)</f>
+        <v>4.971973483132908E-3</v>
+      </c>
+      <c r="AA25">
+        <f>ABS(Y25)</f>
+        <v>1.6807524253678666E-2</v>
+      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>0.01</v>
       </c>
@@ -28718,44 +28742,68 @@
         <f t="shared" si="6"/>
         <v>-3.6955045450972166E-3</v>
       </c>
+      <c r="H26">
+        <f t="shared" ref="H26:H40" si="7">ABS(F26)</f>
+        <v>2.5886414573527972E-3</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ref="I26:I40" si="8">ABS(G26)</f>
+        <v>3.6955045450972166E-3</v>
+      </c>
       <c r="K26">
-        <f t="shared" ref="K26:K41" si="7">K7</f>
+        <f t="shared" ref="K26:K41" si="9">K7</f>
         <v>4.6506582823813121E-3</v>
       </c>
       <c r="L26">
-        <f t="shared" ref="L26:M41" si="8">(L7-L$22)/L$22</f>
+        <f t="shared" ref="L26:M41" si="10">(L7-L$22)/L$22</f>
         <v>4.7068998190760228E-3</v>
       </c>
       <c r="M26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.3567062670319287E-2</v>
       </c>
       <c r="N26">
-        <f t="shared" ref="N26:N41" si="9">N7</f>
+        <f t="shared" ref="N26:N41" si="11">N7</f>
         <v>0.10986676906648206</v>
       </c>
       <c r="O26">
-        <f t="shared" ref="O26:P41" si="10">(O7-O$22)/O$22</f>
+        <f t="shared" ref="O26:P41" si="12">(O7-O$22)/O$22</f>
         <v>4.7067750080677659E-3</v>
       </c>
       <c r="P26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.3566726742124601E-2</v>
       </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26:Q40" si="13">ABS(O26)</f>
+        <v>4.7067750080677659E-3</v>
+      </c>
+      <c r="R26">
+        <f t="shared" ref="R26:R40" si="14">ABS(P26)</f>
+        <v>1.3566726742124601E-2</v>
+      </c>
       <c r="W26">
-        <f t="shared" ref="W26:W41" si="11">W7</f>
+        <f t="shared" ref="W26:W41" si="15">W7</f>
         <v>4.6686864188939678E-2</v>
       </c>
       <c r="X26">
-        <f t="shared" ref="X26:Y41" si="12">(X7-X$22)/X$22</f>
+        <f t="shared" ref="X26:Y41" si="16">(X7-X$22)/X$22</f>
         <v>4.971973483132908E-3</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-1.6807524253678666E-2</v>
       </c>
+      <c r="Z26">
+        <f t="shared" ref="Z26:Z40" si="17">ABS(X26)</f>
+        <v>4.971973483132908E-3</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" ref="AA26:AA40" si="18">ABS(Y26)</f>
+        <v>1.6807524253678666E-2</v>
+      </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1E-3</v>
       </c>
@@ -28783,44 +28831,68 @@
         <f t="shared" si="6"/>
         <v>-1.3626023601002847E-4</v>
       </c>
+      <c r="H27">
+        <f t="shared" si="7"/>
+        <v>9.5379060634657529E-5</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="8"/>
+        <v>1.3626023601002847E-4</v>
+      </c>
       <c r="K27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.6203502806830619E-3</v>
       </c>
       <c r="L27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.5667505557115061E-5</v>
       </c>
       <c r="M27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0287312396664129E-4</v>
       </c>
       <c r="N27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.11688512261085876</v>
       </c>
       <c r="O27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3.5667209785486823E-5</v>
       </c>
       <c r="P27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0287248386223976E-4</v>
       </c>
+      <c r="Q27">
+        <f t="shared" si="13"/>
+        <v>3.5667209785486823E-5</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="14"/>
+        <v>1.0287248386223976E-4</v>
+      </c>
       <c r="W27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.4482831354895588E-2</v>
       </c>
       <c r="X27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-6.6253803985142311E-4</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>2.2946871904753578E-3</v>
       </c>
+      <c r="Z27">
+        <f t="shared" si="17"/>
+        <v>6.6253803985142311E-4</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="18"/>
+        <v>2.2946871904753578E-3</v>
+      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1E-4</v>
       </c>
@@ -28848,44 +28920,68 @@
         <f t="shared" si="6"/>
         <v>-1.3626023601002847E-4</v>
       </c>
+      <c r="H28">
+        <f t="shared" si="7"/>
+        <v>9.5379060634657529E-5</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="8"/>
+        <v>1.3626023601002847E-4</v>
+      </c>
       <c r="K28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.225795198566403E-3</v>
       </c>
       <c r="L28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.5667505557115061E-5</v>
       </c>
       <c r="M28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0287312396664129E-4</v>
       </c>
       <c r="N28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.12633517130185079</v>
       </c>
       <c r="O28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3.5667209785486823E-5</v>
       </c>
       <c r="P28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0287248386223976E-4</v>
       </c>
+      <c r="Q28">
+        <f t="shared" si="13"/>
+        <v>3.5667209785486823E-5</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="14"/>
+        <v>1.0287248386223976E-4</v>
+      </c>
       <c r="W28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.7060253938321537E-2</v>
       </c>
       <c r="X28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-5.7014038052295606E-6</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.9696474555082407E-5</v>
       </c>
+      <c r="Z28">
+        <f t="shared" si="17"/>
+        <v>5.7014038052295606E-6</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="18"/>
+        <v>1.9696474555082407E-5</v>
+      </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f>A28/10</f>
         <v>1.0000000000000001E-5</v>
@@ -28914,46 +29010,70 @@
         <f t="shared" si="6"/>
         <v>1.4801762748213388E-8</v>
       </c>
+      <c r="H29">
+        <f t="shared" si="7"/>
+        <v>1.0360613922730019E-8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="8"/>
+        <v>1.4801762748213388E-8</v>
+      </c>
       <c r="K29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.1212320067930018E-3</v>
       </c>
       <c r="L29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.3863178444663413E-7</v>
       </c>
       <c r="M29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.8419495570976591E-6</v>
       </c>
       <c r="N29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.12460146550721711</v>
       </c>
       <c r="O29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6.3861890089261292E-7</v>
       </c>
       <c r="P29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.8419162070855049E-6</v>
       </c>
+      <c r="Q29">
+        <f t="shared" si="13"/>
+        <v>6.3861890089261292E-7</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="14"/>
+        <v>1.8419162070855049E-6</v>
+      </c>
       <c r="W29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.6198809481958489E-2</v>
       </c>
       <c r="X29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-5.7014038052295606E-6</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.9696474555082407E-5</v>
       </c>
+      <c r="Z29">
+        <f t="shared" si="17"/>
+        <v>5.7014038052295606E-6</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="18"/>
+        <v>1.9696474555082407E-5</v>
+      </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" ref="A30:A40" si="13">A29/10</f>
+        <f t="shared" ref="A30:A40" si="19">A29/10</f>
         <v>1.0000000000000002E-6</v>
       </c>
       <c r="B30">
@@ -28980,46 +29100,70 @@
         <f t="shared" si="6"/>
         <v>1.4801762748213388E-8</v>
       </c>
+      <c r="H30">
+        <f t="shared" si="7"/>
+        <v>1.0360613922730019E-8</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="8"/>
+        <v>1.4801762748213388E-8</v>
+      </c>
       <c r="K30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.7507538014579355E-3</v>
       </c>
       <c r="L30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.3863178444663413E-7</v>
       </c>
       <c r="M30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.8419495570976591E-6</v>
       </c>
       <c r="N30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.13677917125257388</v>
       </c>
       <c r="O30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6.3861890089261292E-7</v>
       </c>
       <c r="P30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.8419162070855049E-6</v>
       </c>
+      <c r="Q30">
+        <f t="shared" si="13"/>
+        <v>6.3861890089261292E-7</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="14"/>
+        <v>1.8419162070855049E-6</v>
+      </c>
       <c r="W30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.1078124629108652E-2</v>
       </c>
       <c r="X30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>3.6541025255175889E-8</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-1.2623437507368986E-7</v>
       </c>
+      <c r="Z30">
+        <f t="shared" si="17"/>
+        <v>3.6541025255175889E-8</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="18"/>
+        <v>1.2623437507368986E-7</v>
+      </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000002E-7</v>
       </c>
       <c r="B31">
@@ -29046,46 +29190,70 @@
         <f t="shared" si="6"/>
         <v>1.4801762748213388E-8</v>
       </c>
+      <c r="H31">
+        <f t="shared" si="7"/>
+        <v>1.0360613922730019E-8</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="8"/>
+        <v>1.4801762748213388E-8</v>
+      </c>
       <c r="K31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.6068291782985706E-3</v>
       </c>
       <c r="L31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.6329441409254097E-10</v>
       </c>
       <c r="M31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.7097397228821172E-10</v>
       </c>
       <c r="N31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.14619977398726192</v>
       </c>
       <c r="O31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.6328995277378418E-10</v>
       </c>
       <c r="P31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.7096324224818246E-10</v>
       </c>
+      <c r="Q31">
+        <f t="shared" si="13"/>
+        <v>1.6328995277378418E-10</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="14"/>
+        <v>4.7096324224818246E-10</v>
+      </c>
       <c r="W31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.0660172330956927E-2</v>
       </c>
       <c r="X31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>3.6541025255175889E-8</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-1.2623437507368986E-7</v>
       </c>
+      <c r="Z31">
+        <f t="shared" si="17"/>
+        <v>3.6541025255175889E-8</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="18"/>
+        <v>1.2623437507368986E-7</v>
+      </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000002E-8</v>
       </c>
       <c r="B32">
@@ -29112,46 +29280,70 @@
         <f t="shared" si="6"/>
         <v>-1.3771374763814781E-8</v>
       </c>
+      <c r="H32">
+        <f t="shared" si="7"/>
+        <v>9.6393858394589124E-9</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="8"/>
+        <v>1.3771374763814781E-8</v>
+      </c>
       <c r="K32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.7735894410406319E-3</v>
       </c>
       <c r="L32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.6329441409254097E-10</v>
       </c>
       <c r="M32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.7097397228821172E-10</v>
       </c>
       <c r="N32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.14362235140383597</v>
       </c>
       <c r="O32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.6328995277378418E-10</v>
       </c>
       <c r="P32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.7096324224818246E-10</v>
       </c>
+      <c r="Q32">
+        <f t="shared" si="13"/>
+        <v>1.6328995277378418E-10</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="14"/>
+        <v>4.7096324224818246E-10</v>
+      </c>
       <c r="W32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.5176821465260826E-2</v>
       </c>
       <c r="X32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0009440308365667E-12</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.4586299845704928E-12</v>
       </c>
+      <c r="Z32">
+        <f t="shared" si="17"/>
+        <v>1.0009440308365667E-12</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="18"/>
+        <v>3.4586299845704928E-12</v>
+      </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000003E-9</v>
       </c>
       <c r="B33">
@@ -29178,46 +29370,70 @@
         <f t="shared" si="6"/>
         <v>-1.8124299825162861E-12</v>
       </c>
+      <c r="H33">
+        <f t="shared" si="7"/>
+        <v>1.2687950447691307E-12</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="8"/>
+        <v>1.8124299825162861E-12</v>
+      </c>
       <c r="K33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.641683575556371E-3</v>
       </c>
       <c r="L33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.6329441409254097E-10</v>
       </c>
       <c r="M33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.7097397228821172E-10</v>
       </c>
       <c r="N33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.14860082130180574</v>
       </c>
       <c r="O33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.6328995277378418E-10</v>
       </c>
       <c r="P33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.7096324224818246E-10</v>
       </c>
+      <c r="Q33">
+        <f t="shared" si="13"/>
+        <v>1.6328995277378418E-10</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="14"/>
+        <v>4.7096324224818246E-10</v>
+      </c>
       <c r="W33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.4794324502250658E-2</v>
       </c>
       <c r="X33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0009440308365667E-12</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.4586299845704928E-12</v>
       </c>
+      <c r="Z33">
+        <f t="shared" si="17"/>
+        <v>1.0009440308365667E-12</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="18"/>
+        <v>3.4586299845704928E-12</v>
+      </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000003E-10</v>
       </c>
       <c r="B34">
@@ -29244,46 +29460,70 @@
         <f t="shared" si="6"/>
         <v>-1.8124299825162861E-12</v>
       </c>
+      <c r="H34">
+        <f t="shared" si="7"/>
+        <v>1.2687950447691307E-12</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="8"/>
+        <v>1.8124299825162861E-12</v>
+      </c>
       <c r="K34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.4623036172554507E-3</v>
       </c>
       <c r="L34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.6705624879068162E-11</v>
       </c>
       <c r="M34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0586681271472334E-10</v>
       </c>
       <c r="N34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.17037250036131391</v>
       </c>
       <c r="O34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3.6710061352562599E-11</v>
       </c>
       <c r="P34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0587979871616332E-10</v>
       </c>
+      <c r="Q34">
+        <f t="shared" si="13"/>
+        <v>3.6710061352562599E-11</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="14"/>
+        <v>1.0587979871616332E-10</v>
+      </c>
       <c r="W34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.5940313046571788E-2</v>
       </c>
       <c r="X34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0009440308365667E-12</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.4586299845704928E-12</v>
       </c>
+      <c r="Z34">
+        <f t="shared" si="17"/>
+        <v>1.0009440308365667E-12</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="18"/>
+        <v>3.4586299845704928E-12</v>
+      </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000003E-11</v>
       </c>
       <c r="B35">
@@ -29310,44 +29550,68 @@
         <f t="shared" si="6"/>
         <v>-1.8124299825162861E-12</v>
       </c>
+      <c r="H35">
+        <f t="shared" si="7"/>
+        <v>1.2687950447691307E-12</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="8"/>
+        <v>1.8124299825162861E-12</v>
+      </c>
       <c r="K35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.5178903715028043E-3</v>
       </c>
       <c r="L35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.001397094112364E-16</v>
       </c>
       <c r="M35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.6448074534878007E-15</v>
       </c>
       <c r="N35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.15313009013166851</v>
       </c>
       <c r="O35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.8011170788648664E-16</v>
       </c>
       <c r="P35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9548575343382009E-15</v>
       </c>
+      <c r="Q35">
+        <f t="shared" si="13"/>
+        <v>4.8011170788648664E-16</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="14"/>
+        <v>1.9548575343382009E-15</v>
+      </c>
       <c r="W35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.5818923594053239E-2</v>
       </c>
       <c r="X35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0009440308365667E-12</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.4586299845704928E-12</v>
       </c>
+      <c r="Z35">
+        <f t="shared" si="17"/>
+        <v>1.0009440308365667E-12</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="18"/>
+        <v>3.4586299845704928E-12</v>
+      </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f>A35/10</f>
         <v>1.0000000000000002E-12</v>
@@ -29376,46 +29640,70 @@
         <f t="shared" si="6"/>
         <v>1.0447598189686741E-12</v>
       </c>
+      <c r="H36">
+        <f t="shared" si="7"/>
+        <v>7.3115428736183662E-13</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="8"/>
+        <v>1.0447598189686741E-12</v>
+      </c>
       <c r="K36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.4872425394312902E-3</v>
       </c>
       <c r="L36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.001397094112364E-16</v>
       </c>
       <c r="M36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.6448074534878007E-15</v>
       </c>
       <c r="N36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.15125035643128229</v>
       </c>
       <c r="O36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.8011170788648664E-16</v>
       </c>
       <c r="P36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9548575343382009E-15</v>
       </c>
+      <c r="Q36">
+        <f t="shared" si="13"/>
+        <v>4.8011170788648664E-16</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="14"/>
+        <v>1.9548575343382009E-15</v>
+      </c>
       <c r="W36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.4125781106573035E-2</v>
       </c>
       <c r="X36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0009440308365667E-12</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.4586299845704928E-12</v>
       </c>
+      <c r="Z36">
+        <f t="shared" si="17"/>
+        <v>1.0009440308365667E-12</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="18"/>
+        <v>3.4586299845704928E-12</v>
+      </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000002E-13</v>
       </c>
       <c r="B37">
@@ -29442,46 +29730,70 @@
         <f t="shared" si="6"/>
         <v>2.3102129191554972E-15</v>
       </c>
+      <c r="H37">
+        <f t="shared" si="7"/>
+        <v>1.4857084833362187E-15</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="8"/>
+        <v>2.3102129191554972E-15</v>
+      </c>
       <c r="K37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.7657772485518146E-3</v>
       </c>
       <c r="L37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.001397094112364E-16</v>
       </c>
       <c r="M37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.6448074534878007E-15</v>
       </c>
       <c r="N37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.23215221996970672</v>
       </c>
       <c r="O37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.8011170788648664E-16</v>
       </c>
       <c r="P37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9548575343382009E-15</v>
       </c>
+      <c r="Q37">
+        <f t="shared" si="13"/>
+        <v>4.8011170788648664E-16</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="14"/>
+        <v>1.9548575343382009E-15</v>
+      </c>
       <c r="W37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>7.003179862811891E-2</v>
       </c>
       <c r="X37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>4.7626202894681991E-16</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-2.428244782052768E-15</v>
       </c>
+      <c r="Z37">
+        <f t="shared" si="17"/>
+        <v>4.7626202894681991E-16</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="18"/>
+        <v>2.428244782052768E-15</v>
+      </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000002E-14</v>
       </c>
       <c r="B38">
@@ -29508,46 +29820,70 @@
         <f t="shared" si="6"/>
         <v>2.3102129191554972E-15</v>
       </c>
+      <c r="H38">
+        <f t="shared" si="7"/>
+        <v>1.4857084833362187E-15</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="8"/>
+        <v>2.3102129191554972E-15</v>
+      </c>
       <c r="K38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.654002802173352E-3</v>
       </c>
       <c r="L38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.001397094112364E-16</v>
       </c>
       <c r="M38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.6448074534878007E-15</v>
       </c>
       <c r="N38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.14919935543402588</v>
       </c>
       <c r="O38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.8011170788648664E-16</v>
       </c>
       <c r="P38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9548575343382009E-15</v>
       </c>
+      <c r="Q38">
+        <f t="shared" si="13"/>
+        <v>4.8011170788648664E-16</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="14"/>
+        <v>1.9548575343382009E-15</v>
+      </c>
       <c r="W38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.8616890380817336E-2</v>
       </c>
       <c r="X38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>4.7626202894681991E-16</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-2.428244782052768E-15</v>
       </c>
+      <c r="Z38">
+        <f t="shared" si="17"/>
+        <v>4.7626202894681991E-16</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="18"/>
+        <v>2.428244782052768E-15</v>
+      </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000001E-15</v>
       </c>
       <c r="B39">
@@ -29574,46 +29910,70 @@
         <f t="shared" si="6"/>
         <v>-6.7947438798691086E-16</v>
       </c>
+      <c r="H39">
+        <f t="shared" si="7"/>
+        <v>5.5714068125108201E-16</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="8"/>
+        <v>6.7947438798691086E-16</v>
+      </c>
       <c r="K39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.6248573148112257E-3</v>
       </c>
       <c r="L39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.001397094112364E-16</v>
       </c>
       <c r="M39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2.6448074534878007E-15</v>
       </c>
       <c r="N39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.15075338080141676</v>
       </c>
       <c r="O39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.8011170788648664E-16</v>
       </c>
       <c r="P39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.9548575343382009E-15</v>
       </c>
+      <c r="Q39">
+        <f t="shared" si="13"/>
+        <v>4.8011170788648664E-16</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="14"/>
+        <v>1.9548575343382009E-15</v>
+      </c>
       <c r="W39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>7.5554117310887098E-2</v>
       </c>
       <c r="X39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-1.5875400964893999E-15</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>5.0588432959432672E-15</v>
       </c>
+      <c r="Z39">
+        <f t="shared" si="17"/>
+        <v>1.5875400964893999E-15</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="18"/>
+        <v>5.0588432959432672E-15</v>
+      </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000001E-16</v>
       </c>
       <c r="B40">
@@ -29640,44 +30000,68 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K40">
+      <c r="H40">
         <f t="shared" si="7"/>
-        <v>4.0091570914726612E-3</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="8"/>
-        <v>2.4005588376449458E-16</v>
-      </c>
-      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N40">
+      <c r="K40">
         <f t="shared" si="9"/>
-        <v>0.17083552300074725</v>
-      </c>
-      <c r="O40">
+        <v>4.0091570914726612E-3</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="10"/>
-        <v>2.4005585394324332E-16</v>
-      </c>
-      <c r="P40">
+        <v>2.4005588376449458E-16</v>
+      </c>
+      <c r="M40">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+      <c r="N40">
+        <f t="shared" si="11"/>
+        <v>0.17083552300074725</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="12"/>
+        <v>2.4005585394324332E-16</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="13"/>
+        <v>2.4005585394324332E-16</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="W40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>8.9813171416629936E-2</v>
       </c>
       <c r="X40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.5875400964893999E-16</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-1.214122391026384E-15</v>
       </c>
+      <c r="Z40">
+        <f t="shared" si="17"/>
+        <v>1.5875400964893999E-16</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="18"/>
+        <v>1.214122391026384E-15</v>
+      </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -29706,40 +30090,153 @@
         <v>0</v>
       </c>
       <c r="K41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.0010444300419669E-3</v>
       </c>
       <c r="L41">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <f t="shared" si="9"/>
-        <v>0.20261522157631415</v>
-      </c>
-      <c r="O41">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P41">
+      <c r="M41">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="W41">
+      <c r="N41">
         <f t="shared" si="11"/>
-        <v>8.4745161773980657E-2</v>
-      </c>
-      <c r="X41">
+        <v>0.20261522157631415</v>
+      </c>
+      <c r="O41">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Y41">
+      <c r="P41">
         <f t="shared" si="12"/>
         <v>0</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="15"/>
+        <v>8.4745161773980657E-2</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>900</v>
+      </c>
+      <c r="C50">
+        <v>7390</v>
+      </c>
+      <c r="D50">
+        <v>1.5</v>
+      </c>
+      <c r="E50">
+        <v>290</v>
+      </c>
+      <c r="F50">
+        <v>7390</v>
+      </c>
+      <c r="G50">
+        <v>1.5</v>
+      </c>
+      <c r="H50">
+        <v>1210</v>
+      </c>
+      <c r="I50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>600</v>
+      </c>
+      <c r="C51">
+        <v>7390</v>
+      </c>
+      <c r="D51">
+        <v>1.5</v>
+      </c>
+      <c r="E51">
+        <v>290</v>
+      </c>
+      <c r="F51">
+        <v>7390</v>
+      </c>
+      <c r="G51">
+        <v>0.5</v>
+      </c>
+      <c r="H51">
+        <v>1210</v>
+      </c>
+      <c r="I51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>800</v>
+      </c>
+      <c r="C52">
+        <v>4800</v>
+      </c>
+      <c r="D52">
+        <v>1.5</v>
+      </c>
+      <c r="E52">
+        <v>400</v>
+      </c>
+      <c r="F52">
+        <v>4800</v>
+      </c>
+      <c r="G52">
+        <v>0.5</v>
+      </c>
+      <c r="H52">
+        <v>1210</v>
+      </c>
+      <c r="I52" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -29766,16 +30263,17 @@
   <dimension ref="A1:AB109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
+      <selection pane="bottomRight" activeCell="Y60" sqref="Y60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -32249,7 +32747,7 @@
         <v>561.81977250656314</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>45</v>
       </c>
@@ -32299,7 +32797,7 @@
         <v>561.81974390160269</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>46</v>
       </c>
@@ -32349,7 +32847,7 @@
         <v>561.81971705649073</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>47</v>
       </c>
@@ -32399,7 +32897,7 @@
         <v>561.81969199766093</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>48</v>
       </c>
@@ -32449,7 +32947,7 @@
         <v>561.81966840131167</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>49</v>
       </c>
@@ -32499,7 +32997,7 @@
         <v>561.81964624716227</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>50</v>
       </c>
@@ -32549,7 +33047,7 @@
         <v>561.81962540210566</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>100</v>
       </c>
@@ -32599,7 +33097,7 @@
         <v>561.81924491007635</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -32612,12 +33110,16 @@
         <v>-2.411178384407274E-2</v>
       </c>
       <c r="F60">
-        <f t="shared" ref="F60:G79" si="1">(F5-F$55)/F$55</f>
+        <f>(F5-F$55)/F$55</f>
         <v>1.696796581265415E-2</v>
       </c>
       <c r="G60">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F60:G79" si="1">(G5-G$55)/G$55</f>
         <v>-2.4111818746183455E-2</v>
+      </c>
+      <c r="H60">
+        <f>ABS(G60)</f>
+        <v>2.4111818746183455E-2</v>
       </c>
       <c r="L60">
         <f t="shared" ref="L60:M79" si="2">(L5-L$55)/L$55</f>
@@ -32635,6 +33137,10 @@
         <f t="shared" si="3"/>
         <v>-5.9679714247145764E-2</v>
       </c>
+      <c r="Q60">
+        <f>ABS(P60)</f>
+        <v>5.9679714247145764E-2</v>
+      </c>
       <c r="X60">
         <f t="shared" ref="X60:Y60" si="4">(X5-X$55)/X$55</f>
         <v>-2.5434953787057293E-3</v>
@@ -32643,8 +33149,16 @@
         <f t="shared" si="4"/>
         <v>8.8705145283724442E-3</v>
       </c>
+      <c r="Z60">
+        <f>ABS(X60)</f>
+        <v>2.5434953787057293E-3</v>
+      </c>
+      <c r="AA60">
+        <f>ABS(Y60)</f>
+        <v>8.8705145283724442E-3</v>
+      </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -32664,6 +33178,10 @@
         <f t="shared" si="1"/>
         <v>-2.0874709191333295E-3</v>
       </c>
+      <c r="H61">
+        <f t="shared" ref="H61:H109" si="5">ABS(G61)</f>
+        <v>2.0874709191333295E-3</v>
+      </c>
       <c r="L61">
         <f t="shared" si="2"/>
         <v>2.6655595795035888E-3</v>
@@ -32680,16 +33198,28 @@
         <f t="shared" si="3"/>
         <v>-7.6847314733117181E-3</v>
       </c>
+      <c r="Q61">
+        <f t="shared" ref="Q61:Q109" si="6">ABS(P61)</f>
+        <v>7.6847314733117181E-3</v>
+      </c>
       <c r="X61">
-        <f t="shared" ref="X61:Y61" si="5">(X6-X$55)/X$55</f>
+        <f t="shared" ref="X61:Y61" si="7">(X6-X$55)/X$55</f>
         <v>1.0477948043440132E-3</v>
       </c>
       <c r="Y61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-3.6044826803450863E-3</v>
       </c>
+      <c r="Z61">
+        <f t="shared" ref="Z61:Z79" si="8">ABS(X61)</f>
+        <v>1.0477948043440132E-3</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" ref="AA61:AA79" si="9">ABS(Y61)</f>
+        <v>3.6044826803450863E-3</v>
+      </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -32709,6 +33239,10 @@
         <f t="shared" si="1"/>
         <v>-8.9831377058131336E-4</v>
       </c>
+      <c r="H62">
+        <f t="shared" si="5"/>
+        <v>8.9831377058131336E-4</v>
+      </c>
       <c r="L62">
         <f t="shared" si="2"/>
         <v>1.0433407211824252E-3</v>
@@ -32725,16 +33259,28 @@
         <f t="shared" si="3"/>
         <v>-3.0086021274756299E-3</v>
       </c>
+      <c r="Q62">
+        <f t="shared" si="6"/>
+        <v>3.0086021274756299E-3</v>
+      </c>
       <c r="X62">
-        <f t="shared" ref="X62:Y62" si="6">(X7-X$55)/X$55</f>
+        <f t="shared" ref="X62:Y62" si="10">(X7-X$55)/X$55</f>
         <v>-2.435452844984881E-4</v>
       </c>
       <c r="Y62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8.4214732456841838E-4</v>
       </c>
+      <c r="Z62">
+        <f t="shared" si="8"/>
+        <v>2.435452844984881E-4</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="9"/>
+        <v>8.4214732456841838E-4</v>
+      </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4</v>
       </c>
@@ -32754,6 +33300,10 @@
         <f t="shared" si="1"/>
         <v>-4.1954047886178436E-4</v>
       </c>
+      <c r="H63">
+        <f t="shared" si="5"/>
+        <v>4.1954047886178436E-4</v>
+      </c>
       <c r="L63">
         <f t="shared" si="2"/>
         <v>5.4818207766033176E-4</v>
@@ -32770,16 +33320,28 @@
         <f t="shared" si="3"/>
         <v>-1.5808070652940441E-3</v>
       </c>
+      <c r="Q63">
+        <f t="shared" si="6"/>
+        <v>1.5808070652940441E-3</v>
+      </c>
       <c r="X63">
-        <f t="shared" ref="X63:Y63" si="7">(X8-X$55)/X$55</f>
+        <f t="shared" ref="X63:Y63" si="11">(X8-X$55)/X$55</f>
         <v>6.0287729147139979E-5</v>
       </c>
       <c r="Y63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-2.0821907713811834E-4</v>
       </c>
+      <c r="Z63">
+        <f t="shared" si="8"/>
+        <v>6.0287729147139979E-5</v>
+      </c>
+      <c r="AA63">
+        <f t="shared" si="9"/>
+        <v>2.0821907713811834E-4</v>
+      </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5</v>
       </c>
@@ -32799,6 +33361,10 @@
         <f t="shared" si="1"/>
         <v>-3.3774113815794121E-4</v>
       </c>
+      <c r="H64">
+        <f t="shared" si="5"/>
+        <v>3.3774113815794121E-4</v>
+      </c>
       <c r="L64">
         <f t="shared" si="2"/>
         <v>3.2790265220581104E-4</v>
@@ -32815,16 +33381,28 @@
         <f t="shared" si="3"/>
         <v>-9.4562684026770804E-4</v>
       </c>
+      <c r="Q64">
+        <f t="shared" si="6"/>
+        <v>9.4562684026770804E-4</v>
+      </c>
       <c r="X64">
-        <f t="shared" ref="X64:Y64" si="8">(X9-X$55)/X$55</f>
+        <f t="shared" ref="X64:Y64" si="12">(X9-X$55)/X$55</f>
         <v>-4.81176199340617E-5</v>
       </c>
       <c r="Y64">
+        <f t="shared" si="12"/>
+        <v>1.6625734670848487E-4</v>
+      </c>
+      <c r="Z64">
         <f t="shared" si="8"/>
+        <v>4.81176199340617E-5</v>
+      </c>
+      <c r="AA64">
+        <f t="shared" si="9"/>
         <v>1.6625734670848487E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>6</v>
       </c>
@@ -32844,6 +33422,10 @@
         <f t="shared" si="1"/>
         <v>-2.5463380717398687E-4</v>
       </c>
+      <c r="H65">
+        <f t="shared" si="5"/>
+        <v>2.5463380717398687E-4</v>
+      </c>
       <c r="L65">
         <f t="shared" si="2"/>
         <v>2.4416374089463464E-4</v>
@@ -32860,16 +33442,28 @@
         <f t="shared" si="3"/>
         <v>-7.0416251959919075E-4</v>
       </c>
+      <c r="Q65">
+        <f t="shared" si="6"/>
+        <v>7.0416251959919075E-4</v>
+      </c>
       <c r="X65">
-        <f t="shared" ref="X65:Y65" si="9">(X10-X$55)/X$55</f>
+        <f t="shared" ref="X65:Y65" si="13">(X10-X$55)/X$55</f>
         <v>4.5417616973851829E-6</v>
       </c>
       <c r="Y65">
+        <f t="shared" si="13"/>
+        <v>-1.5689576881724087E-5</v>
+      </c>
+      <c r="Z65">
+        <f t="shared" si="8"/>
+        <v>4.5417616973851829E-6</v>
+      </c>
+      <c r="AA65">
         <f t="shared" si="9"/>
-        <v>-1.5689576881724087E-5</v>
+        <v>1.5689576881724087E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7</v>
       </c>
@@ -32889,6 +33483,10 @@
         <f t="shared" si="1"/>
         <v>-1.7372689440023283E-4</v>
       </c>
+      <c r="H66">
+        <f t="shared" si="5"/>
+        <v>1.7372689440023283E-4</v>
+      </c>
       <c r="L66">
         <f t="shared" si="2"/>
         <v>1.8805344786634103E-4</v>
@@ -32905,16 +33503,28 @@
         <f t="shared" si="3"/>
         <v>-5.4231702762739945E-4</v>
       </c>
+      <c r="Q66">
+        <f t="shared" si="6"/>
+        <v>5.4231702762739945E-4</v>
+      </c>
       <c r="X66">
-        <f t="shared" ref="X66:Y66" si="10">(X11-X$55)/X$55</f>
+        <f t="shared" ref="X66:Y66" si="14">(X11-X$55)/X$55</f>
         <v>-2.3093730741796684E-5</v>
       </c>
       <c r="Y66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7.9786267274323074E-5</v>
       </c>
+      <c r="Z66">
+        <f t="shared" si="8"/>
+        <v>2.3093730741796684E-5</v>
+      </c>
+      <c r="AA66">
+        <f t="shared" si="9"/>
+        <v>7.9786267274323074E-5</v>
+      </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>8</v>
       </c>
@@ -32934,6 +33544,10 @@
         <f t="shared" si="1"/>
         <v>-1.2355927262703545E-4</v>
       </c>
+      <c r="H67">
+        <f t="shared" si="5"/>
+        <v>1.2355927262703545E-4</v>
+      </c>
       <c r="L67">
         <f t="shared" si="2"/>
         <v>1.4198938369422044E-4</v>
@@ -32950,16 +33564,28 @@
         <f t="shared" si="3"/>
         <v>-4.0947470285047455E-4</v>
       </c>
+      <c r="Q67">
+        <f t="shared" si="6"/>
+        <v>4.0947470285047455E-4</v>
+      </c>
       <c r="X67">
-        <f t="shared" ref="X67:Y67" si="11">(X12-X$55)/X$55</f>
+        <f t="shared" ref="X67:Y67" si="15">(X12-X$55)/X$55</f>
         <v>-2.4067557374710039E-6</v>
       </c>
       <c r="Y67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>8.3143971816770591E-6</v>
       </c>
+      <c r="Z67">
+        <f t="shared" si="8"/>
+        <v>2.4067557374710039E-6</v>
+      </c>
+      <c r="AA67">
+        <f t="shared" si="9"/>
+        <v>8.3143971816770591E-6</v>
+      </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9</v>
       </c>
@@ -32979,6 +33605,10 @@
         <f t="shared" si="1"/>
         <v>-1.0033347771519481E-4</v>
       </c>
+      <c r="H68">
+        <f t="shared" si="5"/>
+        <v>1.0033347771519481E-4</v>
+      </c>
       <c r="L68">
         <f t="shared" si="2"/>
         <v>1.0760415914650271E-4</v>
@@ -32995,16 +33625,28 @@
         <f t="shared" si="3"/>
         <v>-3.1033948975451746E-4</v>
       </c>
+      <c r="Q68">
+        <f t="shared" si="6"/>
+        <v>3.1033948975451746E-4</v>
+      </c>
       <c r="X68">
-        <f t="shared" ref="X68:Y68" si="12">(X13-X$55)/X$55</f>
+        <f t="shared" ref="X68:Y68" si="16">(X13-X$55)/X$55</f>
         <v>-1.0301188406987049E-5</v>
       </c>
       <c r="Y68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>3.5587670064859653E-5</v>
       </c>
+      <c r="Z68">
+        <f t="shared" si="8"/>
+        <v>1.0301188406987049E-5</v>
+      </c>
+      <c r="AA68">
+        <f t="shared" si="9"/>
+        <v>3.5587670064859653E-5</v>
+      </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>10</v>
       </c>
@@ -33024,6 +33666,10 @@
         <f t="shared" si="1"/>
         <v>-8.3487741041967165E-5</v>
       </c>
+      <c r="H69">
+        <f t="shared" si="5"/>
+        <v>8.3487741041967165E-5</v>
+      </c>
       <c r="L69">
         <f t="shared" si="2"/>
         <v>8.4719084544044264E-5</v>
@@ -33040,16 +33686,28 @@
         <f t="shared" si="3"/>
         <v>-2.4433546955527019E-4</v>
       </c>
+      <c r="Q69">
+        <f t="shared" si="6"/>
+        <v>2.4433546955527019E-4</v>
+      </c>
       <c r="X69">
-        <f t="shared" ref="X69:Y69" si="13">(X14-X$55)/X$55</f>
+        <f t="shared" ref="X69:Y69" si="17">(X14-X$55)/X$55</f>
         <v>-4.9620273458832865E-6</v>
       </c>
       <c r="Y69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1.7142030612341475E-5</v>
       </c>
+      <c r="Z69">
+        <f t="shared" si="8"/>
+        <v>4.9620273458832865E-6</v>
+      </c>
+      <c r="AA69">
+        <f t="shared" si="9"/>
+        <v>1.7142030612341475E-5</v>
+      </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>11</v>
       </c>
@@ -33069,6 +33727,10 @@
         <f t="shared" si="1"/>
         <v>-6.7760364619009859E-5</v>
       </c>
+      <c r="H70">
+        <f t="shared" si="5"/>
+        <v>6.7760364619009859E-5</v>
+      </c>
       <c r="L70">
         <f t="shared" si="2"/>
         <v>7.0423571007294074E-5</v>
@@ -33085,16 +33747,28 @@
         <f t="shared" si="3"/>
         <v>-2.0310426669184795E-4</v>
       </c>
+      <c r="Q70">
+        <f t="shared" si="6"/>
+        <v>2.0310426669184795E-4</v>
+      </c>
       <c r="X70">
-        <f t="shared" ref="X70:Y70" si="14">(X15-X$55)/X$55</f>
+        <f t="shared" ref="X70:Y70" si="18">(X15-X$55)/X$55</f>
         <v>-4.6450677718519795E-6</v>
       </c>
       <c r="Y70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1.604702860299561E-5</v>
       </c>
+      <c r="Z70">
+        <f t="shared" si="8"/>
+        <v>4.6450677718519795E-6</v>
+      </c>
+      <c r="AA70">
+        <f t="shared" si="9"/>
+        <v>1.604702860299561E-5</v>
+      </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>12</v>
       </c>
@@ -33114,6 +33788,10 @@
         <f t="shared" si="1"/>
         <v>-5.5692159345920798E-5</v>
       </c>
+      <c r="H71">
+        <f t="shared" si="5"/>
+        <v>5.5692159345920798E-5</v>
+      </c>
       <c r="L71">
         <f t="shared" si="2"/>
         <v>5.9910793887680063E-5</v>
@@ -33130,16 +33808,28 @@
         <f t="shared" si="3"/>
         <v>-1.7278422568574886E-4</v>
       </c>
+      <c r="Q71">
+        <f t="shared" si="6"/>
+        <v>1.7278422568574886E-4</v>
+      </c>
       <c r="X71">
-        <f t="shared" ref="X71:Y71" si="15">(X16-X$55)/X$55</f>
+        <f t="shared" ref="X71:Y71" si="19">(X16-X$55)/X$55</f>
         <v>-4.8860258880325847E-6</v>
       </c>
       <c r="Y71">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1.6879467703305239E-5</v>
       </c>
+      <c r="Z71">
+        <f t="shared" si="8"/>
+        <v>4.8860258880325847E-6</v>
+      </c>
+      <c r="AA71">
+        <f t="shared" si="9"/>
+        <v>1.6879467703305239E-5</v>
+      </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>13</v>
       </c>
@@ -33159,6 +33849,10 @@
         <f t="shared" si="1"/>
         <v>-4.7686118025807678E-5</v>
       </c>
+      <c r="H72">
+        <f t="shared" si="5"/>
+        <v>4.7686118025807678E-5</v>
+      </c>
       <c r="L72">
         <f t="shared" si="2"/>
         <v>5.096074165159463E-5</v>
@@ -33175,16 +33869,28 @@
         <f t="shared" si="3"/>
         <v>-1.4697898784297225E-4</v>
       </c>
+      <c r="Q72">
+        <f t="shared" si="6"/>
+        <v>1.4697898784297225E-4</v>
+      </c>
       <c r="X72">
-        <f t="shared" ref="X72:Y72" si="16">(X17-X$55)/X$55</f>
+        <f t="shared" ref="X72:Y72" si="20">(X17-X$55)/X$55</f>
         <v>-2.7413882495322524E-6</v>
       </c>
       <c r="Y72">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>9.4704337302133178E-6</v>
       </c>
+      <c r="Z72">
+        <f t="shared" si="8"/>
+        <v>2.7413882495322524E-6</v>
+      </c>
+      <c r="AA72">
+        <f t="shared" si="9"/>
+        <v>9.4704337302133178E-6</v>
+      </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>14</v>
       </c>
@@ -33204,6 +33910,10 @@
         <f t="shared" si="1"/>
         <v>-4.1493722307679906E-5</v>
       </c>
+      <c r="H73">
+        <f t="shared" si="5"/>
+        <v>4.1493722307679906E-5</v>
+      </c>
       <c r="L73">
         <f t="shared" si="2"/>
         <v>4.3386163865997466E-5</v>
@@ -33220,16 +33930,28 @@
         <f t="shared" si="3"/>
         <v>-1.251206979865966E-4</v>
       </c>
+      <c r="Q73">
+        <f t="shared" si="6"/>
+        <v>1.251206979865966E-4</v>
+      </c>
       <c r="X73">
-        <f t="shared" ref="X73:Y73" si="17">(X18-X$55)/X$55</f>
+        <f t="shared" ref="X73:Y73" si="21">(X18-X$55)/X$55</f>
         <v>-3.838970405338804E-6</v>
       </c>
       <c r="Y73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.3262211823478455E-5</v>
       </c>
+      <c r="Z73">
+        <f t="shared" si="8"/>
+        <v>3.838970405338804E-6</v>
+      </c>
+      <c r="AA73">
+        <f t="shared" si="9"/>
+        <v>1.3262211823478455E-5</v>
+      </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>15</v>
       </c>
@@ -33249,6 +33971,10 @@
         <f t="shared" si="1"/>
         <v>-3.58974384390749E-5</v>
       </c>
+      <c r="H74">
+        <f t="shared" si="5"/>
+        <v>3.58974384390749E-5</v>
+      </c>
       <c r="L74">
         <f t="shared" si="2"/>
         <v>3.7397196644996701E-5</v>
@@ -33265,16 +33991,28 @@
         <f t="shared" si="3"/>
         <v>-1.0784566206996258E-4</v>
       </c>
+      <c r="Q74">
+        <f t="shared" si="6"/>
+        <v>1.0784566206996258E-4</v>
+      </c>
       <c r="X74">
-        <f t="shared" ref="X74:Y74" si="18">(X19-X$55)/X$55</f>
+        <f t="shared" ref="X74:Y74" si="22">(X19-X$55)/X$55</f>
         <v>-2.1393216491368099E-6</v>
       </c>
       <c r="Y74">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>7.390509521199638E-6</v>
       </c>
+      <c r="Z74">
+        <f t="shared" si="8"/>
+        <v>2.1393216491368099E-6</v>
+      </c>
+      <c r="AA74">
+        <f t="shared" si="9"/>
+        <v>7.390509521199638E-6</v>
+      </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>16</v>
       </c>
@@ -33294,6 +34032,10 @@
         <f t="shared" si="1"/>
         <v>-3.1226618971146387E-5</v>
       </c>
+      <c r="H75">
+        <f t="shared" si="5"/>
+        <v>3.1226618971146387E-5</v>
+      </c>
       <c r="L75">
         <f t="shared" si="2"/>
         <v>3.2809428560688541E-5</v>
@@ -33310,16 +34052,28 @@
         <f t="shared" si="3"/>
         <v>-9.4622126408273134E-5</v>
       </c>
+      <c r="Q75">
+        <f t="shared" si="6"/>
+        <v>9.4622126408273134E-5</v>
+      </c>
       <c r="X75">
-        <f t="shared" ref="X75:Y75" si="19">(X20-X$55)/X$55</f>
+        <f t="shared" ref="X75:Y75" si="23">(X20-X$55)/X$55</f>
         <v>-2.8065827832821042E-6</v>
       </c>
       <c r="Y75">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>9.6956580560271225E-6</v>
       </c>
+      <c r="Z75">
+        <f t="shared" si="8"/>
+        <v>2.8065827832821042E-6</v>
+      </c>
+      <c r="AA75">
+        <f t="shared" si="9"/>
+        <v>9.6956580560271225E-6</v>
+      </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>17</v>
       </c>
@@ -33339,6 +34093,10 @@
         <f t="shared" si="1"/>
         <v>-2.7602030148248323E-5</v>
       </c>
+      <c r="H76">
+        <f t="shared" si="5"/>
+        <v>2.7602030148248323E-5</v>
+      </c>
       <c r="L76">
         <f t="shared" si="2"/>
         <v>2.9115390656247394E-5</v>
@@ -33355,16 +34113,28 @@
         <f t="shared" si="3"/>
         <v>-8.3967436750374979E-5</v>
       </c>
+      <c r="Q76">
+        <f t="shared" si="6"/>
+        <v>8.3967436750374979E-5</v>
+      </c>
       <c r="X76">
-        <f t="shared" ref="X76:Y76" si="20">(X21-X$55)/X$55</f>
+        <f t="shared" ref="X76" si="24">(X21-X$55)/X$55</f>
         <v>-1.853824252991266E-6</v>
       </c>
       <c r="Y76">
-        <f t="shared" si="20"/>
+        <f>(Y21-Y$55)/Y$55</f>
         <v>6.4042218351869581E-6</v>
       </c>
+      <c r="Z76">
+        <f t="shared" si="8"/>
+        <v>1.853824252991266E-6</v>
+      </c>
+      <c r="AA76">
+        <f t="shared" si="9"/>
+        <v>6.4042218351869581E-6</v>
+      </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>18</v>
       </c>
@@ -33384,6 +34154,10 @@
         <f t="shared" si="1"/>
         <v>-2.4621271852808246E-5</v>
       </c>
+      <c r="H77">
+        <f t="shared" si="5"/>
+        <v>2.4621271852808246E-5</v>
+      </c>
       <c r="L77">
         <f t="shared" si="2"/>
         <v>2.5913531817012887E-5</v>
@@ -33400,16 +34174,28 @@
         <f t="shared" si="3"/>
         <v>-7.4736212522209612E-5</v>
       </c>
+      <c r="Q77">
+        <f t="shared" si="6"/>
+        <v>7.4736212522209612E-5</v>
+      </c>
       <c r="X77">
-        <f t="shared" ref="X77:Y77" si="21">(X22-X$55)/X$55</f>
+        <f t="shared" ref="X77:Y77" si="25">(X22-X$55)/X$55</f>
         <v>-2.059151213081015E-6</v>
       </c>
       <c r="Y77">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>7.1135501554965363E-6</v>
       </c>
+      <c r="Z77">
+        <f t="shared" si="8"/>
+        <v>2.059151213081015E-6</v>
+      </c>
+      <c r="AA77">
+        <f t="shared" si="9"/>
+        <v>7.1135501554965363E-6</v>
+      </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>19</v>
       </c>
@@ -33429,6 +34215,10 @@
         <f t="shared" si="1"/>
         <v>-2.1979510519327974E-5</v>
       </c>
+      <c r="H78">
+        <f t="shared" si="5"/>
+        <v>2.1979510519327974E-5</v>
+      </c>
       <c r="L78">
         <f t="shared" si="2"/>
         <v>2.3095986432281952E-5</v>
@@ -33445,16 +34235,28 @@
         <f t="shared" si="3"/>
         <v>-6.660882235499295E-5</v>
       </c>
+      <c r="Q78">
+        <f t="shared" si="6"/>
+        <v>6.660882235499295E-5</v>
+      </c>
       <c r="X78">
-        <f t="shared" ref="X78:Y78" si="22">(X23-X$55)/X$55</f>
+        <f t="shared" ref="X78:Y78" si="26">(X23-X$55)/X$55</f>
         <v>-1.6137590341588292E-6</v>
       </c>
       <c r="Y78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>5.5748871954953932E-6</v>
       </c>
+      <c r="Z78">
+        <f t="shared" si="8"/>
+        <v>1.6137590341588292E-6</v>
+      </c>
+      <c r="AA78">
+        <f t="shared" si="9"/>
+        <v>5.5748871954953932E-6</v>
+      </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>20</v>
       </c>
@@ -33474,6 +34276,10 @@
         <f t="shared" si="1"/>
         <v>-1.9712956996151518E-5</v>
       </c>
+      <c r="H79">
+        <f t="shared" si="5"/>
+        <v>1.9712956996151518E-5</v>
+      </c>
       <c r="L79">
         <f t="shared" si="2"/>
         <v>2.0699372448900391E-5</v>
@@ -33490,1362 +34296,1854 @@
         <f t="shared" si="3"/>
         <v>-5.9694892994820865E-5</v>
       </c>
+      <c r="Q79">
+        <f t="shared" si="6"/>
+        <v>5.9694892994820865E-5</v>
+      </c>
       <c r="X79">
-        <f t="shared" ref="X79:Y79" si="23">(X24-X$55)/X$55</f>
+        <f t="shared" ref="X79:Y79" si="27">(X24-X$55)/X$55</f>
         <v>-1.5707475354525977E-6</v>
       </c>
       <c r="Y79">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>5.4262988814683022E-6</v>
       </c>
+      <c r="Z79">
+        <f t="shared" si="8"/>
+        <v>1.5707475354525977E-6</v>
+      </c>
+      <c r="AA79">
+        <f t="shared" si="9"/>
+        <v>5.4262988814683022E-6</v>
+      </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>21</v>
       </c>
       <c r="C80">
-        <f t="shared" ref="C80:D99" si="24">(C25-C$55)/C$55</f>
+        <f t="shared" ref="C80:D99" si="28">(C25-C$55)/C$55</f>
         <v>1.2470274991091947E-5</v>
       </c>
       <c r="D80">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-1.7815124538808162E-5</v>
       </c>
       <c r="F80">
-        <f t="shared" ref="F80:G99" si="25">(F25-F$55)/F$55</f>
+        <f t="shared" ref="F80:G99" si="29">(F25-F$55)/F$55</f>
         <v>1.2469692821867902E-5</v>
       </c>
       <c r="G80">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-1.781439283046783E-5</v>
       </c>
+      <c r="H80">
+        <f t="shared" si="5"/>
+        <v>1.781439283046783E-5</v>
+      </c>
       <c r="L80">
-        <f t="shared" ref="L80:M99" si="26">(L25-L$55)/L$55</f>
+        <f t="shared" ref="L80:M99" si="30">(L25-L$55)/L$55</f>
         <v>1.8690909437750837E-5</v>
       </c>
       <c r="M80">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-5.3904372928301125E-5</v>
       </c>
       <c r="O80">
-        <f t="shared" ref="O80:P99" si="27">(O25-O$55)/O$55</f>
+        <f t="shared" ref="O80:P99" si="31">(O25-O$55)/O$55</f>
         <v>1.8691850863175115E-5</v>
       </c>
       <c r="P80">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-5.3907199688730887E-5</v>
       </c>
+      <c r="Q80">
+        <f t="shared" si="6"/>
+        <v>5.3907199688730887E-5</v>
+      </c>
       <c r="X80">
-        <f t="shared" ref="X80:Y80" si="28">(X25-X$55)/X$55</f>
+        <f t="shared" ref="X80:Y80" si="32">(X25-X$55)/X$55</f>
         <v>-1.3801368001742474E-6</v>
       </c>
       <c r="Y80">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>4.7678121368876298E-6</v>
       </c>
+      <c r="Z80">
+        <f t="shared" ref="Z80:Z109" si="33">ABS(X80)</f>
+        <v>1.3801368001742474E-6</v>
+      </c>
+      <c r="AA80">
+        <f t="shared" ref="AA80:AA109" si="34">ABS(Y80)</f>
+        <v>4.7678121368876298E-6</v>
+      </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>22</v>
       </c>
       <c r="C81">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.1321648747597669E-5</v>
       </c>
       <c r="D81">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-1.6174194129841059E-5</v>
       </c>
       <c r="F81">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.1320703417969758E-5</v>
       </c>
       <c r="G81">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-1.61729344038125E-5</v>
       </c>
+      <c r="H81">
+        <f t="shared" si="5"/>
+        <v>1.61729344038125E-5</v>
+      </c>
       <c r="L81">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.6979191892745263E-5</v>
       </c>
       <c r="M81">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-4.8967809320435105E-5</v>
       </c>
       <c r="O81">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.69808614495692E-5</v>
       </c>
       <c r="P81">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-4.8972725778363683E-5</v>
       </c>
+      <c r="Q81">
+        <f t="shared" si="6"/>
+        <v>4.8972725778363683E-5</v>
+      </c>
       <c r="X81">
-        <f t="shared" ref="X81:Y81" si="29">(X26-X$55)/X$55</f>
+        <f t="shared" ref="X81:Y81" si="35">(X26-X$55)/X$55</f>
         <v>-1.2542014797235016E-6</v>
       </c>
       <c r="Y81">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4.3327546061659508E-6</v>
       </c>
+      <c r="Z81">
+        <f t="shared" si="33"/>
+        <v>1.2542014797235016E-6</v>
+      </c>
+      <c r="AA81">
+        <f t="shared" si="34"/>
+        <v>4.3327546061659508E-6</v>
+      </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>23</v>
       </c>
       <c r="C82">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1.0304578068267035E-5</v>
       </c>
       <c r="D82">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-1.4721203440442003E-5</v>
       </c>
       <c r="F82">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>1.0304081016413881E-5</v>
       </c>
       <c r="G82">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-1.4720575979317219E-5</v>
       </c>
+      <c r="H82">
+        <f t="shared" si="5"/>
+        <v>1.4720575979317219E-5</v>
+      </c>
       <c r="L82">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.5467807112766909E-5</v>
       </c>
       <c r="M82">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-4.4609000148512509E-5</v>
       </c>
       <c r="O82">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.546781244611635E-5</v>
       </c>
       <c r="P82">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-4.4609107972482916E-5</v>
       </c>
+      <c r="Q82">
+        <f t="shared" si="6"/>
+        <v>4.4609107972482916E-5</v>
+      </c>
       <c r="X82">
-        <f t="shared" ref="X82:Y82" si="30">(X27-X$55)/X$55</f>
+        <f t="shared" ref="X82:Y82" si="36">(X27-X$55)/X$55</f>
         <v>-1.1653811394523876E-6</v>
       </c>
       <c r="Y82">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>4.0259151494995145E-6</v>
       </c>
+      <c r="Z82">
+        <f t="shared" si="33"/>
+        <v>1.1653811394523876E-6</v>
+      </c>
+      <c r="AA82">
+        <f t="shared" si="34"/>
+        <v>4.0259151494995145E-6</v>
+      </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>24</v>
       </c>
       <c r="C83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>9.4116760718716631E-6</v>
       </c>
       <c r="D83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-1.3445599865717882E-5</v>
       </c>
       <c r="F83">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>9.4118975845963995E-6</v>
       </c>
       <c r="G83">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-1.3445991798748222E-5</v>
       </c>
+      <c r="H83">
+        <f t="shared" si="5"/>
+        <v>1.3445991798748222E-5</v>
+      </c>
       <c r="L83">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.41198769232051E-5</v>
       </c>
       <c r="M83">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-4.0721589956204554E-5</v>
       </c>
       <c r="O83">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.4119710630198544E-5</v>
       </c>
       <c r="P83">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-4.0721194760126123E-5</v>
       </c>
+      <c r="Q83">
+        <f t="shared" si="6"/>
+        <v>4.0721194760126123E-5</v>
+      </c>
       <c r="X83">
-        <f t="shared" ref="X83:Y83" si="31">(X28-X$55)/X$55</f>
+        <f t="shared" ref="X83:Y83" si="37">(X28-X$55)/X$55</f>
         <v>-1.0384417770346209E-6</v>
       </c>
       <c r="Y83">
-        <f t="shared" si="31"/>
+        <f t="shared" si="37"/>
         <v>3.5873897853423202E-6</v>
       </c>
+      <c r="Z83">
+        <f t="shared" si="33"/>
+        <v>1.0384417770346209E-6</v>
+      </c>
+      <c r="AA83">
+        <f t="shared" si="34"/>
+        <v>3.5873897853423202E-6</v>
+      </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>25</v>
       </c>
       <c r="C84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8.6289597423110836E-6</v>
       </c>
       <c r="D84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-1.2327407465894659E-5</v>
       </c>
       <c r="F84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>8.629067647918781E-6</v>
       </c>
       <c r="G84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-1.2327630825259607E-5</v>
       </c>
+      <c r="H84">
+        <f t="shared" si="5"/>
+        <v>1.2327630825259607E-5</v>
+      </c>
       <c r="L84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.2932809637655907E-5</v>
       </c>
       <c r="M84">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-3.7298104845171134E-5</v>
       </c>
       <c r="O84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.2932565540736221E-5</v>
       </c>
       <c r="P84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-3.7297478168488229E-5</v>
       </c>
+      <c r="Q84">
+        <f t="shared" si="6"/>
+        <v>3.7297478168488229E-5</v>
+      </c>
       <c r="X84">
-        <f t="shared" ref="X84:Y84" si="32">(X29-X$55)/X$55</f>
+        <f t="shared" ref="X84:Y84" si="38">(X29-X$55)/X$55</f>
         <v>-9.8123309226858885E-7</v>
       </c>
       <c r="Y84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>3.3897565162987459E-6</v>
       </c>
+      <c r="Z84">
+        <f t="shared" si="33"/>
+        <v>9.8123309226858885E-7</v>
+      </c>
+      <c r="AA84">
+        <f t="shared" si="34"/>
+        <v>3.3897565162987459E-6</v>
+      </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>26</v>
       </c>
       <c r="C85">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.9317572200748399E-6</v>
       </c>
       <c r="D85">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-1.1331380092073596E-5</v>
       </c>
       <c r="F85">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>7.9322370521657247E-6</v>
       </c>
       <c r="G85">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-1.1332129202078624E-5</v>
       </c>
+      <c r="H85">
+        <f t="shared" si="5"/>
+        <v>1.1332129202078624E-5</v>
+      </c>
       <c r="L85">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.1891806635112061E-5</v>
       </c>
       <c r="M85">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-3.4295866198100229E-5</v>
       </c>
       <c r="O85">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.1891461329188899E-5</v>
       </c>
       <c r="P85">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-3.4294941414293838E-5</v>
       </c>
+      <c r="Q85">
+        <f t="shared" si="6"/>
+        <v>3.4294941414293838E-5</v>
+      </c>
       <c r="X85">
-        <f t="shared" ref="X85:Y85" si="33">(X30-X$55)/X$55</f>
+        <f t="shared" ref="X85:Y85" si="39">(X30-X$55)/X$55</f>
         <v>-8.799654992708384E-7</v>
       </c>
       <c r="Y85">
+        <f t="shared" si="39"/>
+        <v>3.0399174476710701E-6</v>
+      </c>
+      <c r="Z85">
         <f t="shared" si="33"/>
+        <v>8.799654992708384E-7</v>
+      </c>
+      <c r="AA85">
+        <f t="shared" si="34"/>
         <v>3.0399174476710701E-6</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>27</v>
       </c>
       <c r="C86">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>7.314511688570226E-6</v>
       </c>
       <c r="D86">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-1.044957938581933E-5</v>
       </c>
       <c r="F86">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>7.3146504301917424E-6</v>
       </c>
       <c r="G86">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-1.0449836260699346E-5</v>
       </c>
+      <c r="H86">
+        <f t="shared" si="5"/>
+        <v>1.0449836260699346E-5</v>
+      </c>
       <c r="L86">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.0968905444395415E-5</v>
       </c>
       <c r="M86">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-3.1634230925943002E-5</v>
       </c>
       <c r="O86">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.0969190437298177E-5</v>
       </c>
       <c r="P86">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-3.1635118405096266E-5</v>
       </c>
+      <c r="Q86">
+        <f t="shared" si="6"/>
+        <v>3.1635118405096266E-5</v>
+      </c>
       <c r="X86">
-        <f t="shared" ref="X86:Y86" si="34">(X31-X$55)/X$55</f>
+        <f t="shared" ref="X86:Y86" si="40">(X31-X$55)/X$55</f>
         <v>-8.3025893347836103E-7</v>
       </c>
       <c r="Y86">
+        <f t="shared" si="40"/>
+        <v>2.8682012277497218E-6</v>
+      </c>
+      <c r="Z86">
+        <f t="shared" si="33"/>
+        <v>8.3025893347836103E-7</v>
+      </c>
+      <c r="AA86">
         <f t="shared" si="34"/>
         <v>2.8682012277497218E-6</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>28</v>
       </c>
       <c r="C87">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>6.7625573733198563E-6</v>
       </c>
       <c r="D87">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-9.6610538431272676E-6</v>
       </c>
       <c r="F87">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>6.763099007078874E-6</v>
       </c>
       <c r="G87">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-9.6618818705761411E-6</v>
       </c>
+      <c r="H87">
+        <f t="shared" si="5"/>
+        <v>9.6618818705761411E-6</v>
+      </c>
       <c r="L87">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.01389343807214E-5</v>
       </c>
       <c r="M87">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-2.9240604430193543E-5</v>
       </c>
       <c r="O87">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.0138190730608777E-5</v>
       </c>
       <c r="P87">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-2.9238520346324362E-5</v>
       </c>
+      <c r="Q87">
+        <f t="shared" si="6"/>
+        <v>2.9238520346324362E-5</v>
+      </c>
       <c r="X87">
-        <f t="shared" ref="X87:Y87" si="35">(X32-X$55)/X$55</f>
+        <f t="shared" ref="X87:Y87" si="41">(X32-X$55)/X$55</f>
         <v>-7.5560647602171253E-7</v>
       </c>
       <c r="Y87">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>2.6103070962945728E-6</v>
       </c>
+      <c r="Z87">
+        <f t="shared" si="33"/>
+        <v>7.5560647602171253E-7</v>
+      </c>
+      <c r="AA87">
+        <f t="shared" si="34"/>
+        <v>2.6103070962945728E-6</v>
+      </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>29</v>
       </c>
       <c r="C88">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>6.2633993611718729E-6</v>
       </c>
       <c r="D88">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-8.9479532292001473E-6</v>
       </c>
       <c r="F88">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>6.2639225925575688E-6</v>
       </c>
       <c r="G88">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-8.9487509658930909E-6</v>
       </c>
+      <c r="H88">
+        <f t="shared" si="5"/>
+        <v>8.9487509658930909E-6</v>
+      </c>
       <c r="L88">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>9.390177660908144E-6</v>
       </c>
       <c r="M88">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-2.7081198684084048E-5</v>
       </c>
       <c r="O88">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>9.3897727792511562E-6</v>
       </c>
       <c r="P88">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-2.7080087134323853E-5</v>
       </c>
+      <c r="Q88">
+        <f t="shared" si="6"/>
+        <v>2.7080087134323853E-5</v>
+      </c>
       <c r="X88">
-        <f t="shared" ref="X88:Y88" si="36">(X33-X$55)/X$55</f>
+        <f t="shared" ref="X88:Y88" si="42">(X33-X$55)/X$55</f>
         <v>-7.0880126474153587E-7</v>
       </c>
       <c r="Y88">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>2.448614047336998E-6</v>
       </c>
+      <c r="Z88">
+        <f t="shared" si="33"/>
+        <v>7.0880126474153587E-7</v>
+      </c>
+      <c r="AA88">
+        <f t="shared" si="34"/>
+        <v>2.448614047336998E-6</v>
+      </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>30</v>
       </c>
       <c r="C89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>5.8124407609156207E-6</v>
       </c>
       <c r="D89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-8.3037104564117372E-6</v>
       </c>
       <c r="F89">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>5.8122974564064127E-6</v>
       </c>
       <c r="G89">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-8.3035523545959878E-6</v>
       </c>
+      <c r="H89">
+        <f t="shared" si="5"/>
+        <v>8.3035523545959878E-6</v>
+      </c>
       <c r="L89">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>8.71525161183592E-6</v>
       </c>
       <c r="M89">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-2.5134719392101469E-5</v>
       </c>
       <c r="O89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.7155724541353121E-6</v>
       </c>
       <c r="P89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-2.5135696794667642E-5</v>
       </c>
+      <c r="Q89">
+        <f t="shared" si="6"/>
+        <v>2.5135696794667642E-5</v>
+      </c>
       <c r="X89">
-        <f t="shared" ref="X89:Y89" si="37">(X34-X$55)/X$55</f>
+        <f t="shared" ref="X89:Y89" si="43">(X34-X$55)/X$55</f>
         <v>-6.5396321511078596E-7</v>
       </c>
       <c r="Y89">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>2.2591708688585929E-6</v>
       </c>
+      <c r="Z89">
+        <f t="shared" si="33"/>
+        <v>6.5396321511078596E-7</v>
+      </c>
+      <c r="AA89">
+        <f t="shared" si="34"/>
+        <v>2.2591708688585929E-6</v>
+      </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>31</v>
       </c>
       <c r="C90">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>5.4092851958559156E-6</v>
       </c>
       <c r="D90">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-7.7277593131344606E-6</v>
       </c>
       <c r="F90">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>5.4088383691359314E-6</v>
       </c>
       <c r="G90">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-7.727164359468224E-6</v>
       </c>
+      <c r="H90">
+        <f t="shared" si="5"/>
+        <v>7.727164359468224E-6</v>
+      </c>
       <c r="L90">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>8.106885801290323E-6</v>
       </c>
       <c r="M90">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-2.3380198814197052E-5</v>
       </c>
       <c r="O90">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.1071826173543461E-6</v>
       </c>
       <c r="P90">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-2.3381103287137349E-5</v>
       </c>
+      <c r="Q90">
+        <f t="shared" si="6"/>
+        <v>2.3381103287137349E-5</v>
+      </c>
       <c r="X90">
-        <f t="shared" ref="X90:Y90" si="38">(X35-X$55)/X$55</f>
+        <f t="shared" ref="X90:Y90" si="44">(X35-X$55)/X$55</f>
         <v>-6.1108673330260285E-7</v>
       </c>
       <c r="Y90">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>2.1110501035577559E-6</v>
       </c>
+      <c r="Z90">
+        <f t="shared" si="33"/>
+        <v>6.1108673330260285E-7</v>
+      </c>
+      <c r="AA90">
+        <f t="shared" si="34"/>
+        <v>2.1110501035577559E-6</v>
+      </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>32</v>
       </c>
       <c r="C91">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>5.042803915329673E-6</v>
       </c>
       <c r="D91">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-7.2042012183914855E-6</v>
       </c>
       <c r="F91">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>5.0426088375365407E-6</v>
       </c>
       <c r="G91">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-7.2039629788016728E-6</v>
       </c>
+      <c r="H91">
+        <f t="shared" si="5"/>
+        <v>7.2039629788016728E-6</v>
+      </c>
       <c r="L91">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>7.5539015815273919E-6</v>
       </c>
       <c r="M91">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-2.1785397925095278E-5</v>
       </c>
       <c r="O91">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>7.5543573318356755E-6</v>
       </c>
       <c r="P91">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-2.1786757458389984E-5</v>
       </c>
+      <c r="Q91">
+        <f t="shared" si="6"/>
+        <v>2.1786757458389984E-5</v>
+      </c>
       <c r="X91">
-        <f t="shared" ref="X91:Y91" si="39">(X36-X$55)/X$55</f>
+        <f t="shared" ref="X91:Y91" si="45">(X36-X$55)/X$55</f>
         <v>-5.6918052606036663E-7</v>
       </c>
       <c r="Y91">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>1.9662812913779157E-6</v>
       </c>
+      <c r="Z91">
+        <f t="shared" si="33"/>
+        <v>5.6918052606036663E-7</v>
+      </c>
+      <c r="AA91">
+        <f t="shared" si="34"/>
+        <v>1.9662812913779157E-6</v>
+      </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>33</v>
       </c>
       <c r="C92">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>4.7040250232897674E-6</v>
       </c>
       <c r="D92">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-6.7202188797732988E-6</v>
       </c>
       <c r="F92">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>4.7045958746708576E-6</v>
       </c>
       <c r="G92">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-6.7210721431617572E-6</v>
       </c>
+      <c r="H92">
+        <f t="shared" si="5"/>
+        <v>6.7210721431617572E-6</v>
+      </c>
       <c r="L92">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>7.0504523114080624E-6</v>
       </c>
       <c r="M92">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-2.0333455135390859E-5</v>
       </c>
       <c r="O92">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>7.0508138383136808E-6</v>
       </c>
       <c r="P92">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-2.0334539920431418E-5</v>
       </c>
+      <c r="Q92">
+        <f t="shared" si="6"/>
+        <v>2.0334539920431418E-5</v>
+      </c>
       <c r="X92">
-        <f t="shared" ref="X92:Y92" si="40">(X37-X$55)/X$55</f>
+        <f t="shared" ref="X92:Y92" si="46">(X37-X$55)/X$55</f>
         <v>-5.3145968279259116E-7</v>
       </c>
       <c r="Y92">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>1.8359712411194124E-6</v>
       </c>
+      <c r="Z92">
+        <f t="shared" si="33"/>
+        <v>5.3145968279259116E-7</v>
+      </c>
+      <c r="AA92">
+        <f t="shared" si="34"/>
+        <v>1.8359712411194124E-6</v>
+      </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>34</v>
       </c>
       <c r="C93">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>4.3972006026031445E-6</v>
       </c>
       <c r="D93">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-6.2818868840695891E-6</v>
       </c>
       <c r="F93">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>4.3973131584782601E-6</v>
       </c>
       <c r="G93">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-6.2820829581369752E-6</v>
       </c>
+      <c r="H93">
+        <f t="shared" si="5"/>
+        <v>6.2820829581369752E-6</v>
+      </c>
       <c r="L93">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>6.5925730430217517E-6</v>
       </c>
       <c r="M93">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-1.9012935626571245E-5</v>
       </c>
       <c r="O93">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>6.5925469836263502E-6</v>
       </c>
       <c r="P93">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-1.9012899876684182E-5</v>
       </c>
+      <c r="Q93">
+        <f t="shared" si="6"/>
+        <v>1.9012899876684182E-5</v>
+      </c>
       <c r="X93">
-        <f t="shared" ref="X93:Y93" si="41">(X38-X$55)/X$55</f>
+        <f t="shared" ref="X93:Y93" si="47">(X38-X$55)/X$55</f>
         <v>-4.9777820385733789E-7</v>
       </c>
       <c r="Y93">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>1.7196155706204399E-6</v>
       </c>
+      <c r="Z93">
+        <f t="shared" si="33"/>
+        <v>4.9777820385733789E-7</v>
+      </c>
+      <c r="AA93">
+        <f t="shared" si="34"/>
+        <v>1.7196155706204399E-6</v>
+      </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>35</v>
       </c>
       <c r="C94">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>4.1187078516380418E-6</v>
       </c>
       <c r="D94">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-5.8840296871356317E-6</v>
       </c>
       <c r="F94">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>4.1193519484077173E-6</v>
       </c>
       <c r="G94">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-5.8849828973630346E-6</v>
       </c>
+      <c r="H94">
+        <f t="shared" si="5"/>
+        <v>5.8849828973630346E-6</v>
+      </c>
       <c r="L94">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>6.17275052908311E-6</v>
       </c>
       <c r="M94">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-1.780217130582395E-5</v>
       </c>
       <c r="O94">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>6.1731326312881518E-6</v>
       </c>
       <c r="P94">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-1.7803310183894624E-5</v>
       </c>
+      <c r="Q94">
+        <f t="shared" si="6"/>
+        <v>1.7803310183894624E-5</v>
+      </c>
       <c r="X94">
-        <f t="shared" ref="X94:Y94" si="42">(X39-X$55)/X$55</f>
+        <f t="shared" ref="X94:Y94" si="48">(X39-X$55)/X$55</f>
         <v>-4.6560134511844252E-7</v>
       </c>
       <c r="Y94">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>1.6084577732573779E-6</v>
       </c>
+      <c r="Z94">
+        <f t="shared" si="33"/>
+        <v>4.6560134511844252E-7</v>
+      </c>
+      <c r="AA94">
+        <f t="shared" si="34"/>
+        <v>1.6084577732573779E-6</v>
+      </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>36</v>
       </c>
       <c r="C95">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.8624560493072747E-6</v>
       </c>
       <c r="D95">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-5.5179460506672673E-6</v>
       </c>
       <c r="F95">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.8625517507984664E-6</v>
       </c>
       <c r="G95">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-5.5181137578337459E-6</v>
       </c>
+      <c r="H95">
+        <f t="shared" si="5"/>
+        <v>5.5181137578337459E-6</v>
+      </c>
       <c r="L95">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>5.7868218269320687E-6</v>
       </c>
       <c r="M95">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-1.668915631845242E-5</v>
       </c>
       <c r="O95">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>5.787144892853765E-6</v>
       </c>
       <c r="P95">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-1.6690122629848443E-5</v>
       </c>
+      <c r="Q95">
+        <f t="shared" si="6"/>
+        <v>1.6690122629848443E-5</v>
+      </c>
       <c r="X95">
-        <f t="shared" ref="X95:Y95" si="43">(X40-X$55)/X$55</f>
+        <f t="shared" ref="X95:Y95" si="49">(X40-X$55)/X$55</f>
         <v>-4.3745926510970345E-7</v>
       </c>
       <c r="Y95">
-        <f t="shared" si="43"/>
+        <f t="shared" si="49"/>
         <v>1.5112384985223135E-6</v>
       </c>
+      <c r="Z95">
+        <f t="shared" si="33"/>
+        <v>4.3745926510970345E-7</v>
+      </c>
+      <c r="AA95">
+        <f t="shared" si="34"/>
+        <v>1.5112384985223135E-6</v>
+      </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>37</v>
       </c>
       <c r="C96">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.6238724166665781E-6</v>
       </c>
       <c r="D96">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-5.177103272117148E-6</v>
       </c>
       <c r="F96">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.623693171829446E-6</v>
       </c>
       <c r="G96">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-5.176876272840071E-6</v>
       </c>
+      <c r="H96">
+        <f t="shared" si="5"/>
+        <v>5.176876272840071E-6</v>
+      </c>
       <c r="L96">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>5.4312053429141246E-6</v>
       </c>
       <c r="M96">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-1.5663561403520574E-5</v>
       </c>
       <c r="O96">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>5.4308187488424331E-6</v>
       </c>
       <c r="P96">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-1.5662478933204022E-5</v>
       </c>
+      <c r="Q96">
+        <f t="shared" si="6"/>
+        <v>1.5662478933204022E-5</v>
+      </c>
       <c r="X96">
-        <f t="shared" ref="X96:Y96" si="44">(X41-X$55)/X$55</f>
+        <f t="shared" ref="X96:Y96" si="50">(X41-X$55)/X$55</f>
         <v>-4.1024998393675052E-7</v>
       </c>
       <c r="Y96">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>1.4172416791254509E-6</v>
       </c>
+      <c r="Z96">
+        <f t="shared" si="33"/>
+        <v>4.1024998393675052E-7</v>
+      </c>
+      <c r="AA96">
+        <f t="shared" si="34"/>
+        <v>1.4172416791254509E-6</v>
+      </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>38</v>
       </c>
       <c r="C97">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.4059222679200466E-6</v>
       </c>
       <c r="D97">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-4.8657376385378102E-6</v>
       </c>
       <c r="F97">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.4059105538374423E-6</v>
       </c>
       <c r="G97">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-4.8657482286676897E-6</v>
       </c>
+      <c r="H97">
+        <f t="shared" si="5"/>
+        <v>4.8657482286676897E-6</v>
+      </c>
       <c r="L97">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>5.1035501127257472E-6</v>
       </c>
       <c r="M97">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-1.4718606426940048E-5</v>
       </c>
       <c r="O97">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>5.1034502667429319E-6</v>
       </c>
       <c r="P97">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-1.4718348979350348E-5</v>
       </c>
+      <c r="Q97">
+        <f t="shared" si="6"/>
+        <v>1.4718348979350348E-5</v>
+      </c>
       <c r="X97">
-        <f t="shared" ref="X97:Y97" si="45">(X42-X$55)/X$55</f>
+        <f t="shared" ref="X97:Y97" si="51">(X42-X$55)/X$55</f>
         <v>-3.8617071714345041E-7</v>
       </c>
       <c r="Y97">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>1.3340577819317986E-6</v>
       </c>
+      <c r="Z97">
+        <f t="shared" si="33"/>
+        <v>3.8617071714345041E-7</v>
+      </c>
+      <c r="AA97">
+        <f t="shared" si="34"/>
+        <v>1.3340577819317986E-6</v>
+      </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>39</v>
       </c>
       <c r="C98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.2058064149020901E-6</v>
       </c>
       <c r="D98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-4.5798502141215221E-6</v>
       </c>
       <c r="F98">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.2057838564163863E-6</v>
       </c>
       <c r="G98">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-4.579843705429335E-6</v>
       </c>
+      <c r="H98">
+        <f t="shared" si="5"/>
+        <v>4.579843705429335E-6</v>
+      </c>
       <c r="L98">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>4.8025562527007577E-6</v>
       </c>
       <c r="M98">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-1.3850542552300932E-5</v>
       </c>
       <c r="O98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>4.8023734825356976E-6</v>
       </c>
       <c r="P98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-1.3850044152914314E-5</v>
       </c>
+      <c r="Q98">
+        <f t="shared" si="6"/>
+        <v>1.3850044152914314E-5</v>
+      </c>
       <c r="X98">
-        <f t="shared" ref="X98:Y98" si="46">(X43-X$55)/X$55</f>
+        <f t="shared" ref="X98:Y98" si="52">(X43-X$55)/X$55</f>
         <v>-3.631398949501546E-7</v>
       </c>
       <c r="Y98">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>1.2544958413251229E-6</v>
       </c>
+      <c r="Z98">
+        <f t="shared" si="33"/>
+        <v>3.631398949501546E-7</v>
+      </c>
+      <c r="AA98">
+        <f t="shared" si="34"/>
+        <v>1.2544958413251229E-6</v>
+      </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>40</v>
       </c>
       <c r="C99">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.018396435359552E-6</v>
       </c>
       <c r="D99">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-4.3121144918685009E-6</v>
       </c>
       <c r="F99">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.0186099842240241E-6</v>
       </c>
       <c r="G99">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-4.3124437875903592E-6</v>
       </c>
+      <c r="H99">
+        <f t="shared" si="5"/>
+        <v>4.3124437875903592E-6</v>
+      </c>
       <c r="L99">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>4.5233136047282122E-6</v>
       </c>
       <c r="M99">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-1.3045208940256076E-5</v>
       </c>
       <c r="O99">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>4.5232529365309049E-6</v>
       </c>
       <c r="P99">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-1.3045061014140536E-5</v>
       </c>
+      <c r="Q99">
+        <f t="shared" si="6"/>
+        <v>1.3045061014140536E-5</v>
+      </c>
       <c r="X99">
-        <f t="shared" ref="X99:Y99" si="47">(X44-X$55)/X$55</f>
+        <f t="shared" ref="X99:Y99" si="53">(X44-X$55)/X$55</f>
         <v>-3.4232247912047572E-7</v>
       </c>
       <c r="Y99">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>1.1825803154562369E-6</v>
       </c>
+      <c r="Z99">
+        <f t="shared" si="33"/>
+        <v>3.4232247912047572E-7</v>
+      </c>
+      <c r="AA99">
+        <f t="shared" si="34"/>
+        <v>1.1825803154562369E-6</v>
+      </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>41</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:D109" si="48">(C45-C$55)/C$55</f>
+        <f t="shared" ref="C100:D109" si="54">(C45-C$55)/C$55</f>
         <v>2.8443459125958802E-6</v>
       </c>
       <c r="D100">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-4.0634641939810253E-6</v>
       </c>
       <c r="F100">
-        <f t="shared" ref="F100:G109" si="49">(F45-F$55)/F$55</f>
+        <f t="shared" ref="F100:G109" si="55">(F45-F$55)/F$55</f>
         <v>2.8441368047802814E-6</v>
       </c>
       <c r="G100">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-4.0631882788811916E-6</v>
       </c>
+      <c r="H100">
+        <f t="shared" si="5"/>
+        <v>4.0631882788811916E-6</v>
+      </c>
       <c r="L100">
-        <f t="shared" ref="L100:M109" si="50">(L45-L$55)/L$55</f>
+        <f t="shared" ref="L100:M109" si="56">(L45-L$55)/L$55</f>
         <v>4.2626340155664125E-6</v>
       </c>
       <c r="M100">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-1.2293410995953798E-5</v>
       </c>
       <c r="O100">
-        <f t="shared" ref="O100:P109" si="51">(O45-O$55)/O$55</f>
+        <f t="shared" ref="O100:P109" si="57">(O45-O$55)/O$55</f>
         <v>4.2630410368982055E-6</v>
       </c>
       <c r="P100">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-1.2294610325652123E-5</v>
       </c>
+      <c r="Q100">
+        <f t="shared" si="6"/>
+        <v>1.2294610325652123E-5</v>
+      </c>
       <c r="X100">
-        <f t="shared" ref="X100:Y100" si="52">(X45-X$55)/X$55</f>
+        <f t="shared" ref="X100:Y100" si="58">(X45-X$55)/X$55</f>
         <v>-3.2267900718341283E-7</v>
       </c>
       <c r="Y100">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1.1147202879572924E-6</v>
       </c>
+      <c r="Z100">
+        <f t="shared" si="33"/>
+        <v>3.2267900718341283E-7</v>
+      </c>
+      <c r="AA100">
+        <f t="shared" si="34"/>
+        <v>1.1147202879572924E-6</v>
+      </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>42</v>
       </c>
       <c r="C101">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>2.6835516161214822E-6</v>
       </c>
       <c r="D101">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-3.8337518510429839E-6</v>
       </c>
       <c r="F101">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2.6839691431046332E-6</v>
       </c>
       <c r="G101">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-3.8343698671381284E-6</v>
       </c>
+      <c r="H101">
+        <f t="shared" si="5"/>
+        <v>3.8343698671381284E-6</v>
+      </c>
       <c r="L101">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>4.02064185090069E-6</v>
       </c>
       <c r="M101">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-1.1595507394357348E-5</v>
       </c>
       <c r="O101">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>4.0205911245953673E-6</v>
       </c>
       <c r="P101">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-1.1595385134397183E-5</v>
       </c>
+      <c r="Q101">
+        <f t="shared" si="6"/>
+        <v>1.1595385134397183E-5</v>
+      </c>
       <c r="X101">
-        <f t="shared" ref="X101:Y101" si="53">(X46-X$55)/X$55</f>
+        <f t="shared" ref="X101:Y101" si="59">(X46-X$55)/X$55</f>
         <v>-3.0456221237265463E-7</v>
       </c>
       <c r="Y101">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1.0521343058205114E-6</v>
       </c>
+      <c r="Z101">
+        <f t="shared" si="33"/>
+        <v>3.0456221237265463E-7</v>
+      </c>
+      <c r="AA101">
+        <f t="shared" si="34"/>
+        <v>1.0521343058205114E-6</v>
+      </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>43</v>
       </c>
       <c r="C102">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>2.534812776093141E-6</v>
       </c>
       <c r="D102">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-3.6212620342040812E-6</v>
       </c>
       <c r="F102">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2.5347843906691965E-6</v>
       </c>
       <c r="G102">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-3.6212418191071839E-6</v>
       </c>
+      <c r="H102">
+        <f t="shared" si="5"/>
+        <v>3.6212418191071839E-6</v>
+      </c>
       <c r="L102">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>3.7962760271180467E-6</v>
       </c>
       <c r="M102">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-1.0948437990525729E-5</v>
       </c>
       <c r="O102">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>3.7962498289658218E-6</v>
       </c>
       <c r="P102">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-1.094838512853137E-5</v>
       </c>
+      <c r="Q102">
+        <f t="shared" si="6"/>
+        <v>1.094838512853137E-5</v>
+      </c>
       <c r="X102">
-        <f t="shared" ref="X102:Y102" si="54">(X47-X$55)/X$55</f>
+        <f t="shared" ref="X102:Y102" si="60">(X47-X$55)/X$55</f>
         <v>-2.8762573129039012E-7</v>
       </c>
       <c r="Y102">
-        <f t="shared" si="54"/>
+        <f t="shared" si="60"/>
         <v>9.9362582207077508E-7</v>
       </c>
+      <c r="Z102">
+        <f t="shared" si="33"/>
+        <v>2.8762573129039012E-7</v>
+      </c>
+      <c r="AA102">
+        <f t="shared" si="34"/>
+        <v>9.9362582207077508E-7</v>
+      </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>44</v>
       </c>
       <c r="C103">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>2.3941665719683385E-6</v>
       </c>
       <c r="D103">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-3.4203334235169695E-6</v>
       </c>
       <c r="F103">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2.3944156035791383E-6</v>
       </c>
       <c r="G103">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-3.4207084024674981E-6</v>
       </c>
+      <c r="H103">
+        <f t="shared" si="5"/>
+        <v>3.4207084024674981E-6</v>
+      </c>
       <c r="L103">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>3.587372129883312E-6</v>
       </c>
       <c r="M103">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-1.0345960636483946E-5</v>
       </c>
       <c r="O103">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>3.5877685823832641E-6</v>
       </c>
       <c r="P103">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-1.0347125451181455E-5</v>
       </c>
+      <c r="Q103">
+        <f t="shared" si="6"/>
+        <v>1.0347125451181455E-5</v>
+      </c>
       <c r="X103">
-        <f t="shared" ref="X103:Y103" si="55">(X48-X$55)/X$55</f>
+        <f t="shared" ref="X103:Y103" si="61">(X48-X$55)/X$55</f>
         <v>-2.7183800622913443E-7</v>
       </c>
       <c r="Y103">
-        <f t="shared" si="55"/>
+        <f t="shared" si="61"/>
         <v>9.3908582087645893E-7</v>
       </c>
+      <c r="Z103">
+        <f t="shared" si="33"/>
+        <v>2.7183800622913443E-7</v>
+      </c>
+      <c r="AA103">
+        <f t="shared" si="34"/>
+        <v>9.3908582087645893E-7</v>
+      </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>45</v>
       </c>
       <c r="C104">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>2.2633248017591432E-6</v>
       </c>
       <c r="D104">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-3.2334115119051498E-6</v>
       </c>
       <c r="F104">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2.2634746921309772E-6</v>
       </c>
       <c r="G104">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-3.233643807113023E-6</v>
       </c>
+      <c r="H104">
+        <f t="shared" si="5"/>
+        <v>3.233643807113023E-6</v>
+      </c>
       <c r="L104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>3.3922001323337496E-6</v>
       </c>
       <c r="M104">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-9.7830859578613895E-6</v>
       </c>
       <c r="O104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>3.3923236676191316E-6</v>
       </c>
       <c r="P104">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-9.7834625111553421E-6</v>
       </c>
+      <c r="Q104">
+        <f t="shared" si="6"/>
+        <v>9.7834625111553421E-6</v>
+      </c>
       <c r="X104">
-        <f t="shared" ref="X104:Y104" si="56">(X49-X$55)/X$55</f>
+        <f t="shared" ref="X104:Y104" si="62">(X49-X$55)/X$55</f>
         <v>-2.5709964511090893E-7</v>
       </c>
       <c r="Y104">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>8.8817093907511007E-7</v>
       </c>
+      <c r="Z104">
+        <f t="shared" si="33"/>
+        <v>2.5709964511090893E-7</v>
+      </c>
+      <c r="AA104">
+        <f t="shared" si="34"/>
+        <v>8.8817093907511007E-7</v>
+      </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>46</v>
       </c>
       <c r="C105">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>2.14202092810812E-6</v>
       </c>
       <c r="D105">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-3.0601155257137532E-6</v>
       </c>
       <c r="F105">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2.1419967362431891E-6</v>
       </c>
       <c r="G105">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-3.0600981517173487E-6</v>
       </c>
+      <c r="H105">
+        <f t="shared" si="5"/>
+        <v>3.0600981517173487E-6</v>
+      </c>
       <c r="L105">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>3.2085818395609662E-6</v>
       </c>
       <c r="M105">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-9.2535320572551171E-6</v>
       </c>
       <c r="O105">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>3.2085350473815236E-6</v>
       </c>
       <c r="P105">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-9.2534162877668965E-6</v>
       </c>
+      <c r="Q105">
+        <f t="shared" si="6"/>
+        <v>9.2534162877668965E-6</v>
+      </c>
       <c r="X105">
-        <f t="shared" ref="X105:Y105" si="57">(X50-X$55)/X$55</f>
+        <f t="shared" ref="X105:Y105" si="63">(X50-X$55)/X$55</f>
         <v>-2.4326802323996476E-7</v>
       </c>
       <c r="Y105">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>8.4038846774799332E-7</v>
       </c>
+      <c r="Z105">
+        <f t="shared" si="33"/>
+        <v>2.4326802323996476E-7</v>
+      </c>
+      <c r="AA105">
+        <f t="shared" si="34"/>
+        <v>8.4038846774799332E-7</v>
+      </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>47</v>
       </c>
       <c r="C106">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>2.0277570761072526E-6</v>
       </c>
       <c r="D106">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-2.8968769792761617E-6</v>
       </c>
       <c r="F106">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>2.0276700378174513E-6</v>
       </c>
       <c r="G106">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-2.8967689034834054E-6</v>
       </c>
+      <c r="H106">
+        <f t="shared" si="5"/>
+        <v>2.8967689034834054E-6</v>
+      </c>
       <c r="L106">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>3.0366484721879426E-6</v>
       </c>
       <c r="M106">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-8.7576773760841918E-6</v>
       </c>
       <c r="O106">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>3.0366697322013223E-6</v>
       </c>
       <c r="P106">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-8.7577568436956839E-6</v>
       </c>
+      <c r="Q106">
+        <f t="shared" si="6"/>
+        <v>8.7577568436956839E-6</v>
+      </c>
       <c r="X106">
-        <f t="shared" ref="X106:Y106" si="58">(X51-X$55)/X$55</f>
+        <f t="shared" ref="X106:Y106" si="64">(X51-X$55)/X$55</f>
         <v>-2.3035676057765824E-7</v>
       </c>
       <c r="Y106">
-        <f t="shared" si="58"/>
+        <f t="shared" si="64"/>
         <v>7.9578545702366636E-7</v>
       </c>
+      <c r="Z106">
+        <f t="shared" si="33"/>
+        <v>2.3035676057765824E-7</v>
+      </c>
+      <c r="AA106">
+        <f t="shared" si="34"/>
+        <v>7.9578545702366636E-7</v>
+      </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>48</v>
       </c>
       <c r="C107">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>1.9197822372636149E-6</v>
       </c>
       <c r="D107">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-2.7426229725733584E-6</v>
       </c>
       <c r="F107">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>1.91974044565005E-6</v>
       </c>
       <c r="G107">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-2.7425786708741301E-6</v>
       </c>
+      <c r="H107">
+        <f t="shared" si="5"/>
+        <v>2.7425786708741301E-6</v>
+      </c>
       <c r="L107">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>2.8765797462507126E-6</v>
       </c>
       <c r="M107">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-8.2960402244991651E-6</v>
       </c>
       <c r="O107">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>2.8763115815634619E-6</v>
       </c>
       <c r="P107">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-8.2952840347576408E-6</v>
       </c>
+      <c r="Q107">
+        <f t="shared" si="6"/>
+        <v>8.2952840347576408E-6</v>
+      </c>
       <c r="X107">
-        <f t="shared" ref="X107:Y107" si="59">(X52-X$55)/X$55</f>
+        <f t="shared" ref="X107:Y107" si="65">(X52-X$55)/X$55</f>
         <v>-2.1819902184478191E-7</v>
       </c>
       <c r="Y107">
-        <f t="shared" si="59"/>
+        <f t="shared" si="65"/>
         <v>7.5378556210159591E-7</v>
       </c>
+      <c r="Z107">
+        <f t="shared" si="33"/>
+        <v>2.1819902184478191E-7</v>
+      </c>
+      <c r="AA107">
+        <f t="shared" si="34"/>
+        <v>7.5378556210159591E-7</v>
+      </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>49</v>
       </c>
       <c r="C108">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>1.8187132258751441E-6</v>
       </c>
       <c r="D108">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-2.5982346958182683E-6</v>
       </c>
       <c r="F108">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>1.8190178406388937E-6</v>
       </c>
       <c r="G108">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-2.5986844662965149E-6</v>
       </c>
+      <c r="H108">
+        <f t="shared" si="5"/>
+        <v>2.5986844662965149E-6</v>
+      </c>
       <c r="L108">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>2.7258137145639107E-6</v>
       </c>
       <c r="M108">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-7.8612319657072251E-6</v>
       </c>
       <c r="O108">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>2.7258017062849841E-6</v>
       </c>
       <c r="P108">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-7.8612136286095699E-6</v>
       </c>
+      <c r="Q108">
+        <f t="shared" si="6"/>
+        <v>7.8612136286095699E-6</v>
+      </c>
       <c r="X108">
-        <f t="shared" ref="X108:Y108" si="60">(X53-X$55)/X$55</f>
+        <f t="shared" ref="X108:Y108" si="66">(X53-X$55)/X$55</f>
         <v>-2.0678435882135624E-7</v>
       </c>
       <c r="Y108">
-        <f t="shared" si="60"/>
+        <f t="shared" si="66"/>
         <v>7.1435268470132653E-7</v>
       </c>
+      <c r="Z108">
+        <f t="shared" si="33"/>
+        <v>2.0678435882135624E-7</v>
+      </c>
+      <c r="AA108">
+        <f t="shared" si="34"/>
+        <v>7.1435268470132653E-7</v>
+      </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>50</v>
       </c>
       <c r="C109">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>1.7247290780362479E-6</v>
       </c>
       <c r="D109">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>-2.4639679243862823E-6</v>
       </c>
       <c r="F109">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>1.7246667082324783E-6</v>
       </c>
       <c r="G109">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>-2.4638926590163507E-6</v>
       </c>
+      <c r="H109">
+        <f t="shared" si="5"/>
+        <v>2.4638926590163507E-6</v>
+      </c>
       <c r="L109">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>2.583502420859972E-6</v>
       </c>
       <c r="M109">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-7.4508070988080686E-6</v>
       </c>
       <c r="O109">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>2.5835595411074015E-6</v>
       </c>
       <c r="P109">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>-7.450987278390224E-6</v>
       </c>
+      <c r="Q109">
+        <f t="shared" si="6"/>
+        <v>7.450987278390224E-6</v>
+      </c>
       <c r="X109">
-        <f t="shared" ref="X109:Y109" si="61">(X54-X$55)/X$55</f>
+        <f t="shared" ref="X109:Y109" si="67">(X54-X$55)/X$55</f>
         <v>-1.960441890891688E-7</v>
       </c>
       <c r="Y109">
-        <f t="shared" si="61"/>
+        <f t="shared" si="67"/>
+        <v>6.7724990333623981E-7</v>
+      </c>
+      <c r="Z109">
+        <f t="shared" si="33"/>
+        <v>1.960441890891688E-7</v>
+      </c>
+      <c r="AA109">
+        <f t="shared" si="34"/>
         <v>6.7724990333623981E-7</v>
       </c>
     </row>
@@ -34872,7 +36170,7 @@
   <dimension ref="C3:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:K6"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>